<commit_message>
add dependency and update agency class name
</commit_message>
<xml_diff>
--- a/Postcode/Queensland.xlsx
+++ b/Postcode/Queensland.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Dropbox/RealestateCrawler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RealestateCrawler\Postcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F0E680-1976-4EAB-AC68-BEF56660A500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -79,6 +80,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -346,2203 +350,2203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4000</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4005</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4006</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4007</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4008</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4009</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4010</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4011</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4012</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4013</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4014</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4017</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4018</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4019</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4020</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4021</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4022</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4025</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4030</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4031</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4032</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4034</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4035</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4036</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>4037</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>4051</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4053</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4054</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4055</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4059</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4060</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4061</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>4064</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>4065</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4066</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>4067</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>4068</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>4069</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>4070</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>4073</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4074</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>4075</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>4076</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>4077</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>4078</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>4101</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>4102</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>4103</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>4104</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>4105</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>4106</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>4107</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>4108</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>4109</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>4110</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>4111</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>4112</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>4113</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>4114</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>4115</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>4116</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>4117</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>4118</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>4119</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>4120</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>4121</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>4122</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>4123</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>4124</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>4125</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>4127</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>4128</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>4129</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>4130</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>4131</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>4132</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>4133</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>4151</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>4152</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>4153</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>4154</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>4155</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>4156</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>4157</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>4158</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>4159</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>4160</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>4161</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>4163</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>4164</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>4165</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>4169</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>4170</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>4171</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>4172</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>4173</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>4174</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>4178</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>4179</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>4183</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>4184</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>4205</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>4207</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>4208</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>4209</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>4210</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>4211</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>4212</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>4213</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>4214</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>4215</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>4216</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>4217</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>4218</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>4220</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>4221</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>4223</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>4224</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>4225</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>4226</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>4227</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>4228</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>4270</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>4272</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>4275</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>4280</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>4285</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>4287</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>4300</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>4301</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>4303</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>4304</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>4305</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>4306</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>4307</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>4309</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>4310</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>4311</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>4312</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>4313</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>4340</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>4341</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>4342</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>4343</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>4344</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>4346</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>4347</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>4350</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>4352</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>4353</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>4354</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>4355</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>4356</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>4357</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>4358</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>4359</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>4360</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>4361</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>4362</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>4363</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>4364</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>4365</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>4370</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>4371</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>4372</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>4373</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>4374</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>4375</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>4376</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>4377</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>4378</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>4380</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>4381</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>4382</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>4383</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>4384</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>4385</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>4387</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>4388</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>4390</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>4400</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>4401</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>4402</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>4403</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>4404</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>4405</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>4406</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>4407</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>4408</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>4410</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>4411</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>4412</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>4413</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>4415</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>4416</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>4417</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>4418</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>4419</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>4420</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>4421</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>4422</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>4423</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>4424</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>4425</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>4426</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>4427</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>4428</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>4454</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>4455</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>4461</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>4462</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>4465</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>4467</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>4468</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>4470</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>4472</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>4474</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>4475</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>4477</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>4478</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>4479</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>4480</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>4481</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>4482</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>4486</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>4487</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>4488</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>4489</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>4490</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>4491</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>4492</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>4493</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>4494</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>4496</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>4497</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>4498</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>4500</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>4501</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>4502</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>4503</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>4504</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>4505</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>4506</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>4507</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>4508</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>4509</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>4510</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>4511</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>4512</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>4514</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>4515</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>4516</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>4517</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>4518</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>4519</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>4520</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>4521</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>4550</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>4551</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>4552</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>4553</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>4554</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>4555</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>4556</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>4557</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>4558</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>4559</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>4560</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>4561</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>4562</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>4563</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>4564</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>4565</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>4566</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>4567</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>4568</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>4569</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>4570</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>4571</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>4572</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>4573</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>4574</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>4575</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>4580</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>4581</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>4600</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>4601</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>4605</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>4606</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>4608</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>4610</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>4611</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>4612</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>4613</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>4614</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>4615</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>4620</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>4621</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>4625</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>4626</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>4627</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>4630</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>4650</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>4655</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>4659</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>4660</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>4662</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>4670</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>4671</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>4673</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>4674</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>4676</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>4677</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>4678</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>4680</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>4694</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>4695</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>4697</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>4699</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>4700</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>4701</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>4702</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>4703</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>4704</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>4705</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>4706</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>4707</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>4709</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>4710</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>4711</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>4712</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>4713</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>4714</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>4715</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>4716</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>4717</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>4718</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>4719</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>4720</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>4721</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>4722</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>4723</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>4724</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>4725</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>4726</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>4727</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>4728</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>4730</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>4731</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>4732</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>4733</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>4735</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>4736</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>4737</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>4738</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>4739</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>4740</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>4741</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>4742</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>4743</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>4744</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>4745</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>4746</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>4750</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>4751</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>4753</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>4754</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>4756</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>4757</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>4798</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>4799</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>4800</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>4801</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>4802</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>4803</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>4804</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>4805</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>4806</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>4807</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>4808</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>4809</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>4810</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>4811</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>4812</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>4813</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>4814</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>4815</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>4816</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>4817</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>4818</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>4819</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>4820</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>4821</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>4822</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>4823</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>4824</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>4825</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>4828</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>4829</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>4830</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>4849</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>4850</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>4852</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>4854</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>4855</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>4856</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>4858</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>4859</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>4860</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>4861</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>4865</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>4868</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>4869</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>4870</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>4871</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>4872</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>4873</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>4874</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>4875</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>4876</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>4877</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>4878</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>4879</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>4880</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>4881</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>4882</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>4883</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>4884</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>4885</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>4886</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>4887</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>4888</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>4890</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>4891</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>4892</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>4895</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A438">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A438">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>